<commit_message>
Functioning duty cycle giving my a resolution of 1ms
</commit_message>
<xml_diff>
--- a/util/delay_calcs.xlsx
+++ b/util/delay_calcs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Prescale</t>
   </si>
@@ -36,16 +36,28 @@
     <t>Increment</t>
   </si>
   <si>
-    <t>Delay (Ideal)</t>
-  </si>
-  <si>
-    <t>Delay (Empirical</t>
-  </si>
-  <si>
-    <t>Register (Empirical</t>
-  </si>
-  <si>
-    <t>Register (Ideal)</t>
+    <t>Scaled Loop</t>
+  </si>
+  <si>
+    <t>Measured Loop</t>
+  </si>
+  <si>
+    <t>Required Loop</t>
+  </si>
+  <si>
+    <t>Delay Counter</t>
+  </si>
+  <si>
+    <t>Chosen Delay</t>
+  </si>
+  <si>
+    <t>Chosen Scale</t>
+  </si>
+  <si>
+    <t>Time shaved per register digit</t>
+  </si>
+  <si>
+    <t>Register Initial value</t>
   </si>
 </sst>
 </file>
@@ -81,9 +93,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -439,20 +452,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -465,17 +483,23 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
       <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
+      <c r="G1" t="s">
+        <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -488,31 +512,43 @@
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="E2" s="2">
-        <f>$B$2/($A$5*C2)</f>
-        <v>1.9531250000000002</v>
-      </c>
-      <c r="F2" s="2">
-        <f>$B$2/($A$6*C2)</f>
-        <v>2.1739130434782608</v>
-      </c>
-      <c r="I2" s="1">
-        <f>256-($A$6/$A$9)</f>
-        <v>25.999999999999972</v>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <f>$A$6*C2</f>
+        <v>4.6000000000000001E-4</v>
+      </c>
+      <c r="G2" s="2">
+        <f>C4</f>
+        <v>8</v>
+      </c>
+      <c r="H2" s="1">
+        <f>(($A$13/G2)/256)*E2</f>
+        <v>3.3203124999999998E-6</v>
+      </c>
+      <c r="I2" s="3">
+        <f>(A13-A15)/H2</f>
+        <v>210.8235294117647</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>4</v>
       </c>
-      <c r="E3" s="2">
-        <f t="shared" ref="E3:E9" si="0">$B$2/($A$5*C3)</f>
-        <v>0.97656250000000011</v>
-      </c>
-      <c r="F3" s="2">
-        <f t="shared" ref="F3:F9" si="1">$B$2/($A$6*C3)</f>
-        <v>1.0869565217391304</v>
-      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="1">
+        <f>$A$6*C3</f>
+        <v>9.2000000000000003E-4</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -522,14 +558,16 @@
       <c r="C4">
         <v>8</v>
       </c>
-      <c r="E4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.48828125000000006</v>
-      </c>
-      <c r="F4" s="2">
-        <f t="shared" si="1"/>
-        <v>0.54347826086956519</v>
-      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="1">
+        <f>$A$6*C4</f>
+        <v>1.8400000000000001E-3</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -540,14 +578,16 @@
       <c r="C5">
         <v>16</v>
       </c>
-      <c r="E5" s="2">
-        <f t="shared" si="0"/>
-        <v>0.24414062500000003</v>
-      </c>
-      <c r="F5" s="2">
-        <f t="shared" si="1"/>
-        <v>0.27173913043478259</v>
-      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="1">
+        <f>$A$6*C5</f>
+        <v>3.6800000000000001E-3</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -557,28 +597,32 @@
       <c r="C6">
         <v>32</v>
       </c>
-      <c r="E6" s="2">
-        <f t="shared" si="0"/>
-        <v>0.12207031250000001</v>
-      </c>
-      <c r="F6" s="2">
-        <f t="shared" si="1"/>
-        <v>0.1358695652173913</v>
-      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="1">
+        <f>$A$6*C6</f>
+        <v>7.3600000000000002E-3</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>64</v>
       </c>
-      <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>6.1035156250000007E-2</v>
-      </c>
-      <c r="F7" s="2">
-        <f t="shared" si="1"/>
-        <v>6.7934782608695649E-2</v>
-      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="1">
+        <f>$A$6*C7</f>
+        <v>1.472E-2</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -588,14 +632,16 @@
       <c r="C8">
         <v>128</v>
       </c>
-      <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>3.0517578125000003E-2</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" si="1"/>
-        <v>3.3967391304347824E-2</v>
-      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="1">
+        <f>$A$6*C8</f>
+        <v>2.9440000000000001E-2</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -606,20 +652,66 @@
       <c r="C9">
         <v>256</v>
       </c>
-      <c r="E9" s="2">
-        <f t="shared" si="0"/>
-        <v>1.5258789062500002E-2</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6983695652173912E-2</v>
-      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="1">
+        <f>$A$6*C9</f>
+        <v>5.8880000000000002E-2</v>
+      </c>
+      <c r="G9" s="2"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>A6/256</f>
         <v>8.9843750000000003E-7</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V1. Made it to a version 1. Not the most accurate at the moment, nor is it fast, but it for the most part reaches spec
</commit_message>
<xml_diff>
--- a/util/delay_calcs.xlsx
+++ b/util/delay_calcs.xlsx
@@ -455,7 +455,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,8 +519,8 @@
         <v>4</v>
       </c>
       <c r="F2" s="1">
-        <f>$A$6*C2</f>
-        <v>4.6000000000000001E-4</v>
+        <f>$A$5*C2</f>
+        <v>5.1199999999999998E-4</v>
       </c>
       <c r="G2" s="2">
         <f>C4</f>
@@ -528,11 +528,11 @@
       </c>
       <c r="H2" s="1">
         <f>(($A$13/G2)/256)*E2</f>
-        <v>3.3203124999999998E-6</v>
+        <v>1.953125E-6</v>
       </c>
       <c r="I2" s="3">
         <f>(A13-A15)/H2</f>
-        <v>210.8235294117647</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -544,8 +544,8 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="1">
-        <f>$A$6*C3</f>
-        <v>9.2000000000000003E-4</v>
+        <f t="shared" ref="F3:F9" si="0">$A$5*C3</f>
+        <v>1.024E-3</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="1"/>
@@ -563,8 +563,8 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="1">
-        <f>$A$6*C4</f>
-        <v>1.8400000000000001E-3</v>
+        <f t="shared" si="0"/>
+        <v>2.0479999999999999E-3</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="1"/>
@@ -583,8 +583,8 @@
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="1">
-        <f>$A$6*C5</f>
-        <v>3.6800000000000001E-3</v>
+        <f t="shared" si="0"/>
+        <v>4.0959999999999998E-3</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="1"/>
@@ -602,8 +602,8 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="1">
-        <f>$A$6*C6</f>
-        <v>7.3600000000000002E-3</v>
+        <f t="shared" si="0"/>
+        <v>8.1919999999999996E-3</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
@@ -618,8 +618,8 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="1">
-        <f>$A$6*C7</f>
-        <v>1.472E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.6383999999999999E-2</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="1"/>
@@ -637,8 +637,8 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="1">
-        <f>$A$6*C8</f>
-        <v>2.9440000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.2767999999999999E-2</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="1"/>
@@ -657,8 +657,8 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="1">
-        <f>$A$6*C9</f>
-        <v>5.8880000000000002E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.5535999999999997E-2</v>
       </c>
       <c r="G9" s="2"/>
       <c r="I9" s="1"/>
@@ -687,7 +687,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1.6999999999999999E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D13">
         <v>12</v>

</xml_diff>